<commit_message>
Added login testcase for Scheduler user, Removed locators from the excel sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/Webelements.xlsx
+++ b/src/main/resources/Webelements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Phoenix-Drogon-Maven\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\phoenix-drogon-maven\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65364766-958B-4087-95D6-698A05553938}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D69FA03-9D87-4BDA-9C15-9F56BE7C2D96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20340" yWindow="-4050" windowWidth="19545" windowHeight="14520" xr2:uid="{E4BED7D3-5CAF-40DE-9B4F-43BCBAA07405}"/>
+    <workbookView xWindow="-4545" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{E4BED7D3-5CAF-40DE-9B4F-43BCBAA07405}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginUsers" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>P@ssw0rd123</t>
   </si>
@@ -134,6 +134,21 @@
   </si>
   <si>
     <t>//body/div[@id='root']/main[@class='main-container remove-overflow-mobile']/section[@class='home home--cus-home d-flex home--margin bg-transparent']/section[@class='home__rightpanel']/article[1]/div[1]</t>
+  </si>
+  <si>
+    <t>pp.sch</t>
+  </si>
+  <si>
+    <t>ja.sch</t>
+  </si>
+  <si>
+    <t>psl.sch</t>
+  </si>
+  <si>
+    <t>pl.sch</t>
+  </si>
+  <si>
+    <t>pp.ic</t>
   </si>
 </sst>
 </file>
@@ -172,7 +187,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -206,12 +221,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -227,9 +268,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -244,6 +282,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -560,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9440FCF-3890-42DA-81B6-5F6A08A53E96}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,32 +640,32 @@
       <c r="E1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
@@ -631,12 +678,12 @@
       <c r="E3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
@@ -651,7 +698,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
@@ -666,7 +713,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
@@ -681,34 +728,58 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A7" s="15"/>
       <c r="B7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="3"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A2:A8"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{9134E4A2-361F-4E1A-93D6-3975DE9A2F3B}"/>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{9134E4A2-361F-4E1A-93D6-3975DE9A2F3B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -717,7 +788,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A9:A12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>